<commit_message>
fixed new track cycle issues + ran all  months from February
</commit_message>
<xml_diff>
--- a/outputs/2024/metric_track_rel-202402.xlsx
+++ b/outputs/2024/metric_track_rel-202402.xlsx
@@ -373,10 +373,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>30.88</v>
+        <v>18.64</v>
       </c>
       <c r="B2">
-        <v>66.91889999999999</v>
+        <v>0.7568</v>
       </c>
     </row>
   </sheetData>
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -431,7 +431,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>92.11</v>
+        <v>78.95</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -439,30 +439,30 @@
         </is>
       </c>
       <c r="E2">
-        <v>16.6688</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IN-JH</t>
+          <t>IN-MN</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jharkhand</t>
+          <t>Manipur</t>
         </is>
       </c>
       <c r="C3">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Jharkhand</t>
+          <t>Manipur</t>
         </is>
       </c>
       <c r="E3">
-        <v>63.6483</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>64</v>
+        <v>49.33</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -485,118 +485,118 @@
         </is>
       </c>
       <c r="E4">
-        <v>29.7385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IN-MZ</t>
+          <t>IN-JH</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mizoram</t>
+          <t>Jharkhand</t>
         </is>
       </c>
       <c r="C5">
-        <v>63.64</v>
+        <v>45.83</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Mizoram</t>
+          <t>Jharkhand</t>
         </is>
       </c>
       <c r="E5">
-        <v>40.022</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IN-PB</t>
+          <t>IN-MZ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Mizoram</t>
         </is>
       </c>
       <c r="C6">
-        <v>63.64</v>
+        <v>36.36</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Mizoram</t>
         </is>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IN-MN</t>
+          <t>IN-NL</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Manipur</t>
+          <t>Nagaland</t>
         </is>
       </c>
       <c r="C7">
-        <v>62.5</v>
+        <v>36.36</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Manipur</t>
+          <t>Nagaland</t>
         </is>
       </c>
       <c r="E7">
-        <v>25</v>
+        <v>33.3333</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IN-ML</t>
+          <t>IN-AR</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Meghalaya</t>
+          <t>Arunachal Pradesh</t>
         </is>
       </c>
       <c r="C8">
-        <v>54.55</v>
+        <v>32</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Meghalaya</t>
+          <t>Arunachal Pradesh</t>
         </is>
       </c>
       <c r="E8">
-        <v>200.055</v>
+        <v>33.3333</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IN-DD</t>
+          <t>IN-PB</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Daman and Diu</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>31.82</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Daman and Diu</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="E9">
@@ -615,7 +615,7 @@
         </is>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -623,333 +623,323 @@
         </is>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>IN-AR</t>
+          <t>IN-JK</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Arunachal Pradesh</t>
+          <t>Jammu and Kashmir</t>
         </is>
       </c>
       <c r="C11">
-        <v>44</v>
+        <v>22.73</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Arunachal Pradesh</t>
+          <t>Jammu and Kashmir</t>
         </is>
       </c>
       <c r="E11">
-        <v>83.33329999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>IN-TR</t>
+          <t>IN-ML</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Tripura</t>
+          <t>Meghalaya</t>
         </is>
       </c>
       <c r="C12">
-        <v>37.5</v>
+        <v>18.18</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Tripura</t>
+          <t>Meghalaya</t>
         </is>
       </c>
       <c r="E12">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>IN-DL</t>
+          <t>IN-TR</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Tripura</t>
         </is>
       </c>
       <c r="C13">
-        <v>36.36</v>
+        <v>12.5</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Tripura</t>
         </is>
       </c>
       <c r="E13">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>IN-HR</t>
+          <t>IN-TS</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Telangana</t>
         </is>
       </c>
       <c r="C14">
-        <v>36.36</v>
+        <v>12.12</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Telangana</t>
         </is>
       </c>
       <c r="E14">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>IN-NL</t>
+          <t>IN-AS</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Nagaland</t>
+          <t>Assam</t>
         </is>
       </c>
       <c r="C15">
-        <v>36.36</v>
+        <v>12.12</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Nagaland</t>
+          <t>Assam</t>
         </is>
       </c>
       <c r="E15">
-        <v>33.3333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>IN-TS</t>
+          <t>IN-HR</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Telangana</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C16">
-        <v>33.33</v>
+        <v>9.09</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Telangana</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="E16">
-        <v>175</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>IN-JK</t>
+          <t>IN-DL</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Jammu and Kashmir</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="C17">
-        <v>31.82</v>
+        <v>9.09</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Jammu and Kashmir</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="E17">
-        <v>39.9912</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>IN-OR</t>
+          <t>IN-HP</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Odisha</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>8.33</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Odisha</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="E18">
-        <v>349.7751</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IN-AS</t>
+          <t>IN-MP</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Assam</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C19">
-        <v>24.24</v>
+        <v>7.69</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Assam</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="E19">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>IN-MP</t>
+          <t>IN-OR</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Odisha</t>
         </is>
       </c>
       <c r="C20">
-        <v>21.15</v>
+        <v>6.67</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Odisha</t>
         </is>
       </c>
       <c r="E20">
-        <v>175.0325</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>IN-WB</t>
+          <t>IN-CT</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>West Bengal</t>
+          <t>Chhattisgarh</t>
         </is>
       </c>
       <c r="C21">
-        <v>13.04</v>
+        <v>3.7</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>West Bengal</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Inf</t>
-        </is>
+          <t>Chhattisgarh</t>
+        </is>
+      </c>
+      <c r="E21">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>IN-RJ</t>
+          <t>IN-DD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Daman and Diu</t>
         </is>
       </c>
       <c r="C22">
-        <v>9.09</v>
+        <v>0</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Inf</t>
-        </is>
+          <t>Daman and Diu</t>
+        </is>
+      </c>
+      <c r="E22">
+        <v>-100</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IN-HP</t>
+          <t>IN-RJ</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C23">
-        <v>8.33</v>
+        <v>0</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
-        </is>
-      </c>
-      <c r="E23">
-        <v>0</v>
+          <t>Rajasthan</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>IN-CT</t>
+          <t>IN-WB</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Chhattisgarh</t>
+          <t>West Bengal</t>
         </is>
       </c>
       <c r="C24">
-        <v>7.41</v>
+        <v>0</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Chhattisgarh</t>
-        </is>
-      </c>
-      <c r="E24">
-        <v>100.2703</v>
+          <t>West Bengal</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -964,28 +954,23 @@
         </is>
       </c>
       <c r="C25">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
           <t>Maharashtra</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Inf</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>IN-CH</t>
+          <t>IN-GJ</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Chandigarh</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C26">
@@ -993,19 +978,19 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Chandigarh</t>
+          <t>Gujarat</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>IN-DN</t>
+          <t>IN-KA</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Dadra and Nagar Haveli</t>
+          <t>Karnataka</t>
         </is>
       </c>
       <c r="C27">
@@ -1013,19 +998,19 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Dadra and Nagar Haveli</t>
+          <t>Karnataka</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>IN-AP</t>
+          <t>IN-TN</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Andhra Pradesh</t>
+          <t>Tamil Nadu</t>
         </is>
       </c>
       <c r="C28">
@@ -1033,67 +1018,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Andhra Pradesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>IN-GJ</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Gujarat</t>
-        </is>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Gujarat</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>IN-TN</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
           <t>Tamil Nadu</t>
-        </is>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Tamil Nadu</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>IN-KA</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
         </is>
       </c>
     </row>
@@ -1134,10 +1059,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>93.33</v>
+        <v>80</v>
       </c>
       <c r="C2">
-        <v>16.6625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1147,7 +1072,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>1.0976</v>
       </c>
     </row>
     <row r="4">
@@ -1157,10 +1085,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>42.61</v>
+        <v>26.96</v>
       </c>
       <c r="C4">
-        <v>68.9532</v>
+        <v>6.8993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>